<commit_message>
All front end AI functions now working, ticker column value added to load financial data function in app.py
</commit_message>
<xml_diff>
--- a/server/financial_analysis_output/comprehensive_financial_analysis.xlsx
+++ b/server/financial_analysis_output/comprehensive_financial_analysis.xlsx
@@ -1008,7 +1008,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1019,368 +1019,423 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>Ticker</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>P/E Ratio</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>EPS</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Market Cap</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Current Price</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Beta</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Volume</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Dividend Yield</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>52 Week Low</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>52 Week High</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>Momentum Score</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr"/>
-      <c r="B2" t="n">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>BMY</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr"/>
+      <c r="C2" t="n">
         <v>-4.41</v>
       </c>
-      <c r="C2" t="n">
+      <c r="D2" t="n">
         <v>124823000000</v>
       </c>
-      <c r="D2" t="n">
+      <c r="E2" t="n">
         <v>63.11</v>
       </c>
-      <c r="E2" t="n">
+      <c r="F2" t="n">
         <v>0.44</v>
       </c>
-      <c r="F2" t="n">
+      <c r="G2" t="n">
         <v>11906520</v>
       </c>
-      <c r="G2" t="n">
+      <c r="H2" t="n">
         <v>3.93</v>
       </c>
-      <c r="H2" t="n">
+      <c r="I2" t="n">
         <v>39.35</v>
       </c>
-      <c r="I2" t="n">
+      <c r="J2" t="n">
         <v>63.33</v>
       </c>
-      <c r="J2" t="n">
+      <c r="K2" t="n">
         <v>0.9908256880733946</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>CME</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
         <v>26.9</v>
       </c>
-      <c r="B3" t="n">
+      <c r="C3" t="n">
         <v>9.68</v>
       </c>
-      <c r="C3" t="n">
+      <c r="D3" t="n">
         <v>93565000000</v>
       </c>
-      <c r="D3" t="n">
+      <c r="E3" t="n">
         <v>262.28</v>
       </c>
-      <c r="E3" t="n">
+      <c r="F3" t="n">
         <v>0.55</v>
       </c>
-      <c r="F3" t="n">
+      <c r="G3" t="n">
         <v>1938693</v>
       </c>
-      <c r="G3" t="n">
+      <c r="H3" t="n">
         <v>4.12</v>
       </c>
-      <c r="H3" t="n">
+      <c r="I3" t="n">
         <v>190.7</v>
       </c>
-      <c r="I3" t="n">
+      <c r="J3" t="n">
         <v>263.65</v>
       </c>
-      <c r="J3" t="n">
+      <c r="K3" t="n">
         <v>0.9812200137080191</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>K</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
         <v>21.19</v>
       </c>
-      <c r="B4" t="n">
+      <c r="C4" t="n">
         <v>3.88</v>
       </c>
-      <c r="C4" t="n">
+      <c r="D4" t="n">
         <v>28387000000</v>
       </c>
-      <c r="D4" t="n">
+      <c r="E4" t="n">
         <v>82.45</v>
       </c>
-      <c r="E4" t="n">
+      <c r="F4" t="n">
         <v>0.33</v>
       </c>
-      <c r="F4" t="n">
+      <c r="G4" t="n">
         <v>2379574</v>
       </c>
-      <c r="G4" t="n">
+      <c r="H4" t="n">
         <v>2.77</v>
       </c>
-      <c r="H4" t="n">
+      <c r="I4" t="n">
         <v>52.46</v>
       </c>
-      <c r="I4" t="n">
+      <c r="J4" t="n">
         <v>83.22</v>
       </c>
-      <c r="J4" t="n">
+      <c r="K4" t="n">
         <v>0.9749674902470743</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="n">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>ABBV</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
         <v>89.73999999999999</v>
       </c>
-      <c r="B5" t="n">
+      <c r="C5" t="n">
         <v>2.38</v>
       </c>
-      <c r="C5" t="n">
+      <c r="D5" t="n">
         <v>377061000000</v>
       </c>
-      <c r="D5" t="n">
+      <c r="E5" t="n">
         <v>216.66</v>
       </c>
-      <c r="E5" t="n">
+      <c r="F5" t="n">
         <v>0.6</v>
       </c>
-      <c r="F5" t="n">
+      <c r="G5" t="n">
         <v>6158467</v>
       </c>
-      <c r="G5" t="n">
+      <c r="H5" t="n">
         <v>3.03</v>
       </c>
-      <c r="H5" t="n">
+      <c r="I5" t="n">
         <v>153.58</v>
       </c>
-      <c r="I5" t="n">
+      <c r="J5" t="n">
         <v>218.66</v>
       </c>
-      <c r="J5" t="n">
+      <c r="K5" t="n">
         <v>0.9692685925015365</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="n">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>MO</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
         <v>8.890000000000001</v>
       </c>
-      <c r="B6" t="n">
+      <c r="C6" t="n">
         <v>6.54</v>
       </c>
-      <c r="C6" t="n">
+      <c r="D6" t="n">
         <v>98312000000</v>
       </c>
-      <c r="D6" t="n">
+      <c r="E6" t="n">
         <v>58.99</v>
       </c>
-      <c r="E6" t="n">
+      <c r="F6" t="n">
         <v>0.61</v>
       </c>
-      <c r="F6" t="n">
+      <c r="G6" t="n">
         <v>8405505</v>
       </c>
-      <c r="G6" t="n">
+      <c r="H6" t="n">
         <v>6.92</v>
       </c>
-      <c r="H6" t="n">
+      <c r="I6" t="n">
         <v>40.65</v>
       </c>
-      <c r="I6" t="n">
+      <c r="J6" t="n">
         <v>59.67</v>
       </c>
-      <c r="J6" t="n">
+      <c r="K6" t="n">
         <v>0.964248159831756</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="n">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>WEC</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
         <v>21.9</v>
       </c>
-      <c r="B7" t="n">
+      <c r="C7" t="n">
         <v>4.83</v>
       </c>
-      <c r="C7" t="n">
+      <c r="D7" t="n">
         <v>33609000000</v>
       </c>
-      <c r="D7" t="n">
+      <c r="E7" t="n">
         <v>108.98</v>
       </c>
-      <c r="E7" t="n">
+      <c r="F7" t="n">
         <v>0.44</v>
       </c>
-      <c r="F7" t="n">
+      <c r="G7" t="n">
         <v>2163967</v>
       </c>
-      <c r="G7" t="n">
+      <c r="H7" t="n">
         <v>3.38</v>
       </c>
-      <c r="H7" t="n">
+      <c r="I7" t="n">
         <v>77.47</v>
       </c>
-      <c r="I7" t="n">
+      <c r="J7" t="n">
         <v>110.19</v>
       </c>
-      <c r="J7" t="n">
+      <c r="K7" t="n">
         <v>0.9630195599022007</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="n">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>KR</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
         <v>18.13</v>
       </c>
-      <c r="B8" t="n">
+      <c r="C8" t="n">
         <v>3.67</v>
       </c>
-      <c r="C8" t="n">
+      <c r="D8" t="n">
         <v>43790000000</v>
       </c>
-      <c r="D8" t="n">
+      <c r="E8" t="n">
         <v>67.72</v>
       </c>
-      <c r="E8" t="n">
+      <c r="F8" t="n">
         <v>0.5</v>
       </c>
-      <c r="F8" t="n">
+      <c r="G8" t="n">
         <v>6392906</v>
       </c>
-      <c r="G8" t="n">
+      <c r="H8" t="n">
         <v>1.92</v>
       </c>
-      <c r="H8" t="n">
+      <c r="I8" t="n">
         <v>49.04</v>
       </c>
-      <c r="I8" t="n">
+      <c r="J8" t="n">
         <v>68.51000000000001</v>
       </c>
-      <c r="J8" t="n">
+      <c r="K8" t="n">
         <v>0.9594247560349252</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="n">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>VRSN</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
         <v>29.53</v>
       </c>
-      <c r="B9" t="n">
+      <c r="C9" t="n">
         <v>8.01</v>
       </c>
-      <c r="C9" t="n">
+      <c r="D9" t="n">
         <v>22377000000</v>
       </c>
-      <c r="D9" t="n">
+      <c r="E9" t="n">
         <v>239.02</v>
       </c>
-      <c r="E9" t="n">
+      <c r="F9" t="n">
         <v>0.87</v>
       </c>
-      <c r="F9" t="n">
+      <c r="G9" t="n">
         <v>782822</v>
       </c>
-      <c r="G9" t="inlineStr"/>
-      <c r="H9" t="n">
+      <c r="H9" t="inlineStr"/>
+      <c r="I9" t="n">
         <v>167.05</v>
       </c>
-      <c r="I9" t="n">
+      <c r="J9" t="n">
         <v>242.23</v>
       </c>
-      <c r="J9" t="n">
+      <c r="K9" t="n">
         <v>0.9573024740622509</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="n">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>GILD</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
         <v>301.13</v>
       </c>
-      <c r="B10" t="n">
+      <c r="C10" t="n">
         <v>0.38</v>
       </c>
-      <c r="C10" t="n">
+      <c r="D10" t="n">
         <v>142505000000</v>
       </c>
-      <c r="D10" t="n">
+      <c r="E10" t="n">
         <v>117.21</v>
       </c>
-      <c r="E10" t="n">
+      <c r="F10" t="n">
         <v>0.24</v>
       </c>
-      <c r="F10" t="n">
+      <c r="G10" t="n">
         <v>7907439</v>
       </c>
-      <c r="G10" t="n">
+      <c r="H10" t="n">
         <v>2.7</v>
       </c>
-      <c r="H10" t="n">
+      <c r="I10" t="n">
         <v>62.07</v>
       </c>
-      <c r="I10" t="n">
+      <c r="J10" t="n">
         <v>119.96</v>
       </c>
-      <c r="J10" t="n">
+      <c r="K10" t="n">
         <v>0.9524961133183624</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="n">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>CBOE</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
         <v>29.29</v>
       </c>
-      <c r="B11" t="n">
+      <c r="C11" t="n">
         <v>7.21</v>
       </c>
-      <c r="C11" t="n">
+      <c r="D11" t="n">
         <v>22109000000</v>
       </c>
-      <c r="D11" t="n">
+      <c r="E11" t="n">
         <v>219.02</v>
       </c>
-      <c r="E11" t="n">
+      <c r="F11" t="n">
         <v>0.66</v>
       </c>
-      <c r="F11" t="n">
+      <c r="G11" t="n">
         <v>801837</v>
       </c>
-      <c r="G11" t="n">
+      <c r="H11" t="n">
         <v>1.15</v>
       </c>
-      <c r="H11" t="n">
+      <c r="I11" t="n">
         <v>166.13</v>
       </c>
-      <c r="I11" t="n">
+      <c r="J11" t="n">
         <v>221.66</v>
       </c>
-      <c r="J11" t="n">
+      <c r="K11" t="n">
         <v>0.9524581307401407</v>
       </c>
     </row>
@@ -1395,7 +1450,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1406,372 +1461,427 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>Ticker</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>P/E Ratio</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>EPS</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Market Cap</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Current Price</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Beta</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Volume</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Dividend Yield</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>52 Week Low</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>52 Week High</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>Momentum Score</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>SITC</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
         <v>1.33</v>
       </c>
-      <c r="B2" t="n">
+      <c r="C2" t="n">
         <v>9.65</v>
       </c>
-      <c r="C2" t="n">
+      <c r="D2" t="n">
         <v>673436000</v>
       </c>
-      <c r="D2" t="n">
+      <c r="E2" t="n">
         <v>13.01</v>
       </c>
-      <c r="E2" t="n">
+      <c r="F2" t="n">
         <v>1.77</v>
       </c>
-      <c r="F2" t="n">
+      <c r="G2" t="n">
         <v>1090997</v>
       </c>
-      <c r="G2" t="n">
+      <c r="H2" t="n">
         <v>16.24</v>
       </c>
-      <c r="H2" t="n">
+      <c r="I2" t="n">
         <v>12.78</v>
       </c>
-      <c r="I2" t="n">
+      <c r="J2" t="n">
         <v>64.44</v>
       </c>
-      <c r="J2" t="n">
+      <c r="K2" t="n">
         <v>0.004452187379016656</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>WU</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
         <v>4.01</v>
       </c>
-      <c r="B3" t="n">
+      <c r="C3" t="n">
         <v>2.74</v>
       </c>
-      <c r="C3" t="n">
+      <c r="D3" t="n">
         <v>3711000000</v>
       </c>
-      <c r="D3" t="n">
+      <c r="E3" t="n">
         <v>11.61</v>
       </c>
-      <c r="E3" t="n">
+      <c r="F3" t="n">
         <v>0.82</v>
       </c>
-      <c r="F3" t="n">
+      <c r="G3" t="n">
         <v>5707334</v>
       </c>
-      <c r="G3" t="n">
+      <c r="H3" t="n">
         <v>8.1</v>
       </c>
-      <c r="H3" t="n">
+      <c r="I3" t="n">
         <v>10.04</v>
       </c>
-      <c r="I3" t="n">
+      <c r="J3" t="n">
         <v>14</v>
       </c>
-      <c r="J3" t="n">
+      <c r="K3" t="n">
         <v>0.3964646464646465</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>AES</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
         <v>5.06</v>
       </c>
-      <c r="B4" t="n">
+      <c r="C4" t="n">
         <v>2.37</v>
       </c>
-      <c r="C4" t="n">
+      <c r="D4" t="n">
         <v>8536000000</v>
       </c>
-      <c r="D4" t="n">
+      <c r="E4" t="n">
         <v>11.78</v>
       </c>
-      <c r="E4" t="n">
+      <c r="F4" t="n">
         <v>0.93</v>
       </c>
-      <c r="F4" t="n">
+      <c r="G4" t="n">
         <v>15210955</v>
       </c>
-      <c r="G4" t="n">
+      <c r="H4" t="n">
         <v>5.81</v>
       </c>
-      <c r="H4" t="n">
+      <c r="I4" t="n">
         <v>9.880000000000001</v>
       </c>
-      <c r="I4" t="n">
+      <c r="J4" t="n">
         <v>22.21</v>
       </c>
-      <c r="J4" t="n">
+      <c r="K4" t="n">
         <v>0.1540957015409569</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="n">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>MTDR</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
         <v>6.58</v>
       </c>
-      <c r="B5" t="n">
+      <c r="C5" t="n">
         <v>7.14</v>
       </c>
-      <c r="C5" t="n">
+      <c r="D5" t="n">
         <v>5885000000</v>
       </c>
-      <c r="D5" t="n">
+      <c r="E5" t="n">
         <v>45.02</v>
       </c>
-      <c r="E5" t="n">
+      <c r="F5" t="n">
         <v>3.18</v>
       </c>
-      <c r="F5" t="n">
+      <c r="G5" t="n">
         <v>1241418</v>
       </c>
-      <c r="G5" t="n">
+      <c r="H5" t="n">
         <v>2.66</v>
       </c>
-      <c r="H5" t="n">
+      <c r="I5" t="n">
         <v>43.89</v>
       </c>
-      <c r="I5" t="n">
+      <c r="J5" t="n">
         <v>71.08</v>
       </c>
-      <c r="J5" t="n">
+      <c r="K5" t="n">
         <v>0.04155939683707255</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="n">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
         <v>6.64</v>
       </c>
-      <c r="B6" t="n">
+      <c r="C6" t="n">
         <v>1.46</v>
       </c>
-      <c r="C6" t="n">
+      <c r="D6" t="n">
         <v>38406000000</v>
       </c>
-      <c r="D6" t="n">
+      <c r="E6" t="n">
         <v>9.960000000000001</v>
       </c>
-      <c r="E6" t="n">
+      <c r="F6" t="n">
         <v>1.61</v>
       </c>
-      <c r="F6" t="n">
+      <c r="G6" t="n">
         <v>84276029</v>
       </c>
-      <c r="G6" t="n">
+      <c r="H6" t="n">
         <v>7.53</v>
       </c>
-      <c r="H6" t="n">
+      <c r="I6" t="n">
         <v>9.06</v>
       </c>
-      <c r="I6" t="n">
+      <c r="J6" t="n">
         <v>14.85</v>
       </c>
-      <c r="J6" t="n">
+      <c r="K6" t="n">
         <v>0.1554404145077721</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="n">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>CALM</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
         <v>6.81</v>
       </c>
-      <c r="B7" t="n">
+      <c r="C7" t="n">
         <v>12.86</v>
       </c>
-      <c r="C7" t="n">
+      <c r="D7" t="n">
         <v>4298000000</v>
       </c>
-      <c r="D7" t="n">
+      <c r="E7" t="n">
         <v>87.37</v>
       </c>
-      <c r="E7" t="n">
+      <c r="F7" t="n">
         <v>-0.13</v>
       </c>
-      <c r="F7" t="n">
+      <c r="G7" t="n">
         <v>916708</v>
       </c>
-      <c r="G7" t="n">
+      <c r="H7" t="n">
         <v>4.9</v>
       </c>
-      <c r="H7" t="n">
+      <c r="I7" t="n">
         <v>55</v>
       </c>
-      <c r="I7" t="n">
+      <c r="J7" t="n">
         <v>116.41</v>
       </c>
-      <c r="J7" t="n">
+      <c r="K7" t="n">
         <v>0.527112848070347</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="n">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>HPE</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
         <v>7.38</v>
       </c>
-      <c r="B8" t="n">
+      <c r="C8" t="n">
         <v>2.08</v>
       </c>
-      <c r="C8" t="n">
+      <c r="D8" t="n">
         <v>20150000000</v>
       </c>
-      <c r="D8" t="n">
+      <c r="E8" t="n">
         <v>15.08</v>
       </c>
-      <c r="E8" t="n">
+      <c r="F8" t="n">
         <v>1.23</v>
       </c>
-      <c r="F8" t="n">
+      <c r="G8" t="n">
         <v>15974187</v>
       </c>
-      <c r="G8" t="n">
+      <c r="H8" t="n">
         <v>3.45</v>
       </c>
-      <c r="H8" t="n">
+      <c r="I8" t="n">
         <v>14.85</v>
       </c>
-      <c r="I8" t="n">
+      <c r="J8" t="n">
         <v>24.66</v>
       </c>
-      <c r="J8" t="n">
+      <c r="K8" t="n">
         <v>0.02344546381243633</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="n">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>DVN</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
         <v>7.55</v>
       </c>
-      <c r="B9" t="n">
+      <c r="C9" t="n">
         <v>4.56</v>
       </c>
-      <c r="C9" t="n">
+      <c r="D9" t="n">
         <v>22317000000</v>
       </c>
-      <c r="D9" t="n">
+      <c r="E9" t="n">
         <v>34.21</v>
       </c>
-      <c r="E9" t="n">
+      <c r="F9" t="n">
         <v>1.95</v>
       </c>
-      <c r="F9" t="n">
+      <c r="G9" t="n">
         <v>10667105</v>
       </c>
-      <c r="G9" t="n">
+      <c r="H9" t="n">
         <v>2.79</v>
       </c>
-      <c r="H9" t="n">
+      <c r="I9" t="n">
         <v>30.39</v>
       </c>
-      <c r="I9" t="n">
+      <c r="J9" t="n">
         <v>55.09</v>
       </c>
-      <c r="J9" t="n">
+      <c r="K9" t="n">
         <v>0.1546558704453441</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="n">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>GM</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
         <v>7.58</v>
       </c>
-      <c r="B10" t="n">
+      <c r="C10" t="n">
         <v>6.37</v>
       </c>
-      <c r="C10" t="n">
+      <c r="D10" t="n">
         <v>48039000000</v>
       </c>
-      <c r="D10" t="n">
+      <c r="E10" t="n">
         <v>48.08</v>
       </c>
-      <c r="E10" t="n">
+      <c r="F10" t="n">
         <v>1.43</v>
       </c>
-      <c r="F10" t="n">
+      <c r="G10" t="n">
         <v>11756725</v>
       </c>
-      <c r="G10" t="n">
+      <c r="H10" t="n">
         <v>1</v>
       </c>
-      <c r="H10" t="n">
+      <c r="I10" t="n">
         <v>38.95</v>
       </c>
-      <c r="I10" t="n">
+      <c r="J10" t="n">
         <v>61.24</v>
       </c>
-      <c r="J10" t="n">
+      <c r="K10" t="n">
         <v>0.4096007178106773</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="n">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>APA</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
         <v>8.460000000000001</v>
       </c>
-      <c r="B11" t="n">
+      <c r="C11" t="n">
         <v>2.27</v>
       </c>
-      <c r="C11" t="n">
+      <c r="D11" t="n">
         <v>6990000000</v>
       </c>
-      <c r="D11" t="n">
+      <c r="E11" t="n">
         <v>19.02</v>
       </c>
-      <c r="E11" t="n">
+      <c r="F11" t="n">
         <v>3.27</v>
       </c>
-      <c r="F11" t="n">
+      <c r="G11" t="n">
         <v>7847306</v>
       </c>
-      <c r="G11" t="n">
+      <c r="H11" t="n">
         <v>5.21</v>
       </c>
-      <c r="H11" t="n">
+      <c r="I11" t="n">
         <v>17.66</v>
       </c>
-      <c r="I11" t="n">
+      <c r="J11" t="n">
         <v>36.05</v>
       </c>
-      <c r="J11" t="n">
+      <c r="K11" t="n">
         <v>0.07395323545405109</v>
       </c>
     </row>
@@ -1786,7 +1896,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1797,368 +1907,423 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>Ticker</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>P/E Ratio</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>EPS</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Market Cap</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Current Price</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Beta</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Volume</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Dividend Yield</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>52 Week Low</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>52 Week High</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>Momentum Score</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>SITC</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
         <v>1.33</v>
       </c>
-      <c r="B2" t="n">
+      <c r="C2" t="n">
         <v>9.65</v>
       </c>
-      <c r="C2" t="n">
+      <c r="D2" t="n">
         <v>673436000</v>
       </c>
-      <c r="D2" t="n">
+      <c r="E2" t="n">
         <v>13.01</v>
       </c>
-      <c r="E2" t="n">
+      <c r="F2" t="n">
         <v>1.77</v>
       </c>
-      <c r="F2" t="n">
+      <c r="G2" t="n">
         <v>1090997</v>
       </c>
-      <c r="G2" t="n">
+      <c r="H2" t="n">
         <v>16.24</v>
       </c>
-      <c r="H2" t="n">
+      <c r="I2" t="n">
         <v>12.78</v>
       </c>
-      <c r="I2" t="n">
+      <c r="J2" t="n">
         <v>64.44</v>
       </c>
-      <c r="J2" t="n">
+      <c r="K2" t="n">
         <v>0.004452187379016656</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>GMRE</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
         <v>871</v>
       </c>
-      <c r="B3" t="n">
+      <c r="C3" t="n">
         <v>0.01</v>
       </c>
-      <c r="C3" t="n">
+      <c r="D3" t="n">
         <v>1184000000</v>
       </c>
-      <c r="D3" t="n">
+      <c r="E3" t="n">
         <v>8.99</v>
       </c>
-      <c r="E3" t="n">
+      <c r="F3" t="n">
         <v>1.3</v>
       </c>
-      <c r="F3" t="n">
+      <c r="G3" t="n">
         <v>537018</v>
       </c>
-      <c r="G3" t="n">
+      <c r="H3" t="n">
         <v>9.34</v>
       </c>
-      <c r="H3" t="n">
+      <c r="I3" t="n">
         <v>7.33</v>
       </c>
-      <c r="I3" t="n">
+      <c r="J3" t="n">
         <v>10.46</v>
       </c>
-      <c r="J3" t="n">
+      <c r="K3" t="n">
         <v>0.5303514376996804</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr"/>
-      <c r="B4" t="n">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>WBA</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr"/>
+      <c r="C4" t="n">
         <v>-10.24</v>
       </c>
-      <c r="C4" t="n">
+      <c r="D4" t="n">
         <v>9694000000</v>
       </c>
-      <c r="D4" t="n">
+      <c r="E4" t="n">
         <v>11.28</v>
       </c>
-      <c r="E4" t="n">
+      <c r="F4" t="n">
         <v>0.6</v>
       </c>
-      <c r="F4" t="n">
+      <c r="G4" t="n">
         <v>27467181</v>
       </c>
-      <c r="G4" t="n">
+      <c r="H4" t="n">
         <v>8.869999999999999</v>
       </c>
-      <c r="H4" t="n">
+      <c r="I4" t="n">
         <v>8.08</v>
       </c>
-      <c r="I4" t="n">
+      <c r="J4" t="n">
         <v>22.05</v>
       </c>
-      <c r="J4" t="n">
+      <c r="K4" t="n">
         <v>0.2290622763063707</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="n">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>WU</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
         <v>4.01</v>
       </c>
-      <c r="B5" t="n">
+      <c r="C5" t="n">
         <v>2.74</v>
       </c>
-      <c r="C5" t="n">
+      <c r="D5" t="n">
         <v>3711000000</v>
       </c>
-      <c r="D5" t="n">
+      <c r="E5" t="n">
         <v>11.61</v>
       </c>
-      <c r="E5" t="n">
+      <c r="F5" t="n">
         <v>0.82</v>
       </c>
-      <c r="F5" t="n">
+      <c r="G5" t="n">
         <v>5707334</v>
       </c>
-      <c r="G5" t="n">
+      <c r="H5" t="n">
         <v>8.1</v>
       </c>
-      <c r="H5" t="n">
+      <c r="I5" t="n">
         <v>10.04</v>
       </c>
-      <c r="I5" t="n">
+      <c r="J5" t="n">
         <v>14</v>
       </c>
-      <c r="J5" t="n">
+      <c r="K5" t="n">
         <v>0.3964646464646465</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="n">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>LADR</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
         <v>13.28</v>
       </c>
-      <c r="B6" t="n">
+      <c r="C6" t="n">
         <v>0.86</v>
       </c>
-      <c r="C6" t="n">
+      <c r="D6" t="n">
         <v>1452000000</v>
       </c>
-      <c r="D6" t="n">
+      <c r="E6" t="n">
         <v>11.7</v>
       </c>
-      <c r="E6" t="n">
+      <c r="F6" t="n">
         <v>1.96</v>
       </c>
-      <c r="F6" t="n">
+      <c r="G6" t="n">
         <v>590867</v>
       </c>
-      <c r="G6" t="n">
+      <c r="H6" t="n">
         <v>8.06</v>
       </c>
-      <c r="H6" t="n">
+      <c r="I6" t="n">
         <v>10.21</v>
       </c>
-      <c r="I6" t="n">
+      <c r="J6" t="n">
         <v>12.48</v>
       </c>
-      <c r="J6" t="n">
+      <c r="K6" t="n">
         <v>0.6563876651982373</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="n">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>GOOD</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
         <v>55.63</v>
       </c>
-      <c r="B7" t="n">
+      <c r="C7" t="n">
         <v>0.27</v>
       </c>
-      <c r="C7" t="n">
+      <c r="D7" t="n">
         <v>670368000</v>
       </c>
-      <c r="D7" t="n">
+      <c r="E7" t="n">
         <v>15.36</v>
       </c>
-      <c r="E7" t="n">
+      <c r="F7" t="n">
         <v>1.24</v>
       </c>
-      <c r="F7" t="n">
+      <c r="G7" t="n">
         <v>329615</v>
       </c>
-      <c r="G7" t="n">
+      <c r="H7" t="n">
         <v>7.99</v>
       </c>
-      <c r="H7" t="n">
+      <c r="I7" t="n">
         <v>12.85</v>
       </c>
-      <c r="I7" t="n">
+      <c r="J7" t="n">
         <v>17.88</v>
       </c>
-      <c r="J7" t="n">
+      <c r="K7" t="n">
         <v>0.4990059642147118</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="n">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
         <v>6.64</v>
       </c>
-      <c r="B8" t="n">
+      <c r="C8" t="n">
         <v>1.46</v>
       </c>
-      <c r="C8" t="n">
+      <c r="D8" t="n">
         <v>38406000000</v>
       </c>
-      <c r="D8" t="n">
+      <c r="E8" t="n">
         <v>9.960000000000001</v>
       </c>
-      <c r="E8" t="n">
+      <c r="F8" t="n">
         <v>1.61</v>
       </c>
-      <c r="F8" t="n">
+      <c r="G8" t="n">
         <v>84276029</v>
       </c>
-      <c r="G8" t="n">
+      <c r="H8" t="n">
         <v>7.53</v>
       </c>
-      <c r="H8" t="n">
+      <c r="I8" t="n">
         <v>9.06</v>
       </c>
-      <c r="I8" t="n">
+      <c r="J8" t="n">
         <v>14.85</v>
       </c>
-      <c r="J8" t="n">
+      <c r="K8" t="n">
         <v>0.1554404145077721</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="n">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>DOW</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
         <v>23.36</v>
       </c>
-      <c r="B9" t="n">
+      <c r="C9" t="n">
         <v>1.57</v>
       </c>
-      <c r="C9" t="n">
+      <c r="D9" t="n">
         <v>25880000000</v>
       </c>
-      <c r="D9" t="n">
+      <c r="E9" t="n">
         <v>37.4</v>
       </c>
-      <c r="E9" t="n">
+      <c r="F9" t="n">
         <v>1.16</v>
       </c>
-      <c r="F9" t="n">
+      <c r="G9" t="n">
         <v>7653336</v>
       </c>
-      <c r="G9" t="n">
+      <c r="H9" t="n">
         <v>7.49</v>
       </c>
-      <c r="H9" t="n">
+      <c r="I9" t="n">
         <v>35.48</v>
       </c>
-      <c r="I9" t="n">
+      <c r="J9" t="n">
         <v>60.69</v>
       </c>
-      <c r="J9" t="n">
+      <c r="K9" t="n">
         <v>0.07616025386751296</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="n">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>LYB</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
         <v>17.86</v>
       </c>
-      <c r="B10" t="n">
+      <c r="C10" t="n">
         <v>4.14</v>
       </c>
-      <c r="C10" t="n">
+      <c r="D10" t="n">
         <v>23922000000</v>
       </c>
-      <c r="D10" t="n">
+      <c r="E10" t="n">
         <v>76.54000000000001</v>
       </c>
-      <c r="E10" t="n">
+      <c r="F10" t="n">
         <v>1.07</v>
       </c>
-      <c r="F10" t="n">
+      <c r="G10" t="n">
         <v>2773958</v>
       </c>
-      <c r="G10" t="n">
+      <c r="H10" t="n">
         <v>7.25</v>
       </c>
-      <c r="H10" t="n">
+      <c r="I10" t="n">
         <v>72.20999999999999</v>
       </c>
-      <c r="I10" t="n">
+      <c r="J10" t="n">
         <v>107.02</v>
       </c>
-      <c r="J10" t="n">
+      <c r="K10" t="n">
         <v>0.124389543234703</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr"/>
-      <c r="B11" t="n">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>KRNY</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr"/>
+      <c r="C11" t="n">
         <v>-1.13</v>
       </c>
-      <c r="C11" t="n">
+      <c r="D11" t="n">
         <v>399103000</v>
       </c>
-      <c r="D11" t="n">
+      <c r="E11" t="n">
         <v>6.23</v>
       </c>
-      <c r="E11" t="n">
+      <c r="F11" t="n">
         <v>0.77</v>
       </c>
-      <c r="F11" t="n">
+      <c r="G11" t="n">
         <v>340681</v>
       </c>
-      <c r="G11" t="n">
+      <c r="H11" t="n">
         <v>7.06</v>
       </c>
-      <c r="H11" t="n">
+      <c r="I11" t="n">
         <v>5.28</v>
       </c>
-      <c r="I11" t="n">
+      <c r="J11" t="n">
         <v>8.59</v>
       </c>
-      <c r="J11" t="n">
+      <c r="K11" t="n">
         <v>0.2870090634441089</v>
       </c>
     </row>
@@ -2173,7 +2338,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2184,360 +2349,415 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>Ticker</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>P/E Ratio</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>EPS</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Market Cap</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Current Price</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Beta</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Volume</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Dividend Yield</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>52 Week Low</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>52 Week High</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>Momentum Score</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr"/>
-      <c r="B2" t="n">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>AKRO</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr"/>
+      <c r="C2" t="n">
         <v>-3.75</v>
       </c>
-      <c r="C2" t="n">
+      <c r="D2" t="n">
         <v>3489000000</v>
       </c>
-      <c r="D2" t="n">
+      <c r="E2" t="n">
         <v>41.68</v>
       </c>
-      <c r="E2" t="n">
+      <c r="F2" t="n">
         <v>-0.2</v>
       </c>
-      <c r="F2" t="n">
+      <c r="G2" t="n">
         <v>1321741</v>
       </c>
-      <c r="G2" t="inlineStr"/>
-      <c r="H2" t="n">
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="n">
         <v>17.86</v>
       </c>
-      <c r="I2" t="n">
+      <c r="J2" t="n">
         <v>58.4</v>
       </c>
-      <c r="J2" t="n">
+      <c r="K2" t="n">
         <v>0.5875678342377899</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>CALM</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
         <v>6.81</v>
       </c>
-      <c r="B3" t="n">
+      <c r="C3" t="n">
         <v>12.86</v>
       </c>
-      <c r="C3" t="n">
+      <c r="D3" t="n">
         <v>4298000000</v>
       </c>
-      <c r="D3" t="n">
+      <c r="E3" t="n">
         <v>87.37</v>
       </c>
-      <c r="E3" t="n">
+      <c r="F3" t="n">
         <v>-0.13</v>
       </c>
-      <c r="F3" t="n">
+      <c r="G3" t="n">
         <v>916708</v>
       </c>
-      <c r="G3" t="n">
+      <c r="H3" t="n">
         <v>4.9</v>
       </c>
-      <c r="H3" t="n">
+      <c r="I3" t="n">
         <v>55</v>
       </c>
-      <c r="I3" t="n">
+      <c r="J3" t="n">
         <v>116.41</v>
       </c>
-      <c r="J3" t="n">
+      <c r="K3" t="n">
         <v>0.527112848070347</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr"/>
-      <c r="B4" t="n">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>STI</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr"/>
+      <c r="C4" t="n">
         <v>-0.37</v>
       </c>
-      <c r="C4" t="n">
+      <c r="D4" t="n">
         <v>16700000</v>
       </c>
-      <c r="D4" t="n">
+      <c r="E4" t="n">
         <v>0.1297</v>
       </c>
-      <c r="E4" t="n">
+      <c r="F4" t="n">
         <v>-0.09</v>
       </c>
-      <c r="F4" t="n">
+      <c r="G4" t="n">
         <v>4779993</v>
       </c>
-      <c r="G4" t="inlineStr"/>
-      <c r="H4" t="n">
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="n">
         <v>0.116</v>
       </c>
-      <c r="I4" t="n">
+      <c r="J4" t="n">
         <v>4.44</v>
       </c>
-      <c r="J4" t="n">
+      <c r="K4" t="n">
         <v>0.00316836262719704</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="n">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>BIIB</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
         <v>12.85</v>
       </c>
-      <c r="B5" t="n">
+      <c r="C5" t="n">
         <v>11.18</v>
       </c>
-      <c r="C5" t="n">
+      <c r="D5" t="n">
         <v>21028000000</v>
       </c>
-      <c r="D5" t="n">
+      <c r="E5" t="n">
         <v>150.71</v>
       </c>
-      <c r="E5" t="n">
+      <c r="F5" t="n">
         <v>0.01</v>
       </c>
-      <c r="F5" t="n">
+      <c r="G5" t="n">
         <v>1578922</v>
       </c>
-      <c r="G5" t="inlineStr"/>
-      <c r="H5" t="n">
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="n">
         <v>128.51</v>
       </c>
-      <c r="I5" t="n">
+      <c r="J5" t="n">
         <v>238</v>
       </c>
-      <c r="J5" t="n">
+      <c r="K5" t="n">
         <v>0.2027582427618962</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="n">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>GIS</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
         <v>13.55</v>
       </c>
-      <c r="B6" t="n">
+      <c r="C6" t="n">
         <v>4.6</v>
       </c>
-      <c r="C6" t="n">
+      <c r="D6" t="n">
         <v>34358000000</v>
       </c>
-      <c r="D6" t="n">
+      <c r="E6" t="n">
         <v>65.3</v>
       </c>
-      <c r="E6" t="n">
+      <c r="F6" t="n">
         <v>0.05</v>
       </c>
-      <c r="F6" t="n">
+      <c r="G6" t="n">
         <v>5017025</v>
       </c>
-      <c r="G6" t="n">
+      <c r="H6" t="n">
         <v>3.68</v>
       </c>
-      <c r="H6" t="n">
+      <c r="I6" t="n">
         <v>55.15</v>
       </c>
-      <c r="I6" t="n">
+      <c r="J6" t="n">
         <v>75.90000000000001</v>
       </c>
-      <c r="J6" t="n">
+      <c r="K6" t="n">
         <v>0.4891566265060239</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="n">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>CPB</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
         <v>23.1</v>
       </c>
-      <c r="B7" t="n">
+      <c r="C7" t="n">
         <v>1.73</v>
       </c>
-      <c r="C7" t="n">
+      <c r="D7" t="n">
         <v>11915000000</v>
       </c>
-      <c r="D7" t="n">
+      <c r="E7" t="n">
         <v>42.04</v>
       </c>
-      <c r="E7" t="n">
+      <c r="F7" t="n">
         <v>0.14</v>
       </c>
-      <c r="F7" t="n">
+      <c r="G7" t="n">
         <v>3225337</v>
       </c>
-      <c r="G7" t="n">
+      <c r="H7" t="n">
         <v>3.9</v>
       </c>
-      <c r="H7" t="n">
+      <c r="I7" t="n">
         <v>36.92</v>
       </c>
-      <c r="I7" t="n">
+      <c r="J7" t="n">
         <v>52.81</v>
       </c>
-      <c r="J7" t="n">
+      <c r="K7" t="n">
         <v>0.3222152297042163</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="n">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>GILD</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
         <v>301.13</v>
       </c>
-      <c r="B8" t="n">
+      <c r="C8" t="n">
         <v>0.38</v>
       </c>
-      <c r="C8" t="n">
+      <c r="D8" t="n">
         <v>142505000000</v>
       </c>
-      <c r="D8" t="n">
+      <c r="E8" t="n">
         <v>117.21</v>
       </c>
-      <c r="E8" t="n">
+      <c r="F8" t="n">
         <v>0.24</v>
       </c>
-      <c r="F8" t="n">
+      <c r="G8" t="n">
         <v>7907439</v>
       </c>
-      <c r="G8" t="n">
+      <c r="H8" t="n">
         <v>2.7</v>
       </c>
-      <c r="H8" t="n">
+      <c r="I8" t="n">
         <v>62.07</v>
       </c>
-      <c r="I8" t="n">
+      <c r="J8" t="n">
         <v>119.96</v>
       </c>
-      <c r="J8" t="n">
+      <c r="K8" t="n">
         <v>0.9524961133183624</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="n">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>CTRA</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
         <v>17.92</v>
       </c>
-      <c r="B9" t="n">
+      <c r="C9" t="n">
         <v>1.5</v>
       </c>
-      <c r="C9" t="n">
+      <c r="D9" t="n">
         <v>20540000000</v>
       </c>
-      <c r="D9" t="n">
+      <c r="E9" t="n">
         <v>26.75</v>
       </c>
-      <c r="E9" t="n">
+      <c r="F9" t="n">
         <v>0.24</v>
       </c>
-      <c r="F9" t="n">
+      <c r="G9" t="n">
         <v>6470532</v>
       </c>
-      <c r="G9" t="n">
+      <c r="H9" t="n">
         <v>3.27</v>
       </c>
-      <c r="H9" t="n">
+      <c r="I9" t="n">
         <v>22.3</v>
       </c>
-      <c r="I9" t="n">
+      <c r="J9" t="n">
         <v>29.95</v>
       </c>
-      <c r="J9" t="n">
+      <c r="K9" t="n">
         <v>0.5816993464052288</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="n">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>REGN</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
         <v>18.72</v>
       </c>
-      <c r="B10" t="n">
+      <c r="C10" t="n">
         <v>38.36</v>
       </c>
-      <c r="C10" t="n">
+      <c r="D10" t="n">
         <v>78513000000</v>
       </c>
-      <c r="D10" t="n">
+      <c r="E10" t="n">
         <v>744.83</v>
       </c>
-      <c r="E10" t="n">
+      <c r="F10" t="n">
         <v>0.27</v>
       </c>
-      <c r="F10" t="n">
+      <c r="G10" t="n">
         <v>917805</v>
       </c>
-      <c r="G10" t="n">
+      <c r="H10" t="n">
         <v>0.47</v>
       </c>
-      <c r="H10" t="n">
+      <c r="I10" t="n">
         <v>642</v>
       </c>
-      <c r="I10" t="n">
+      <c r="J10" t="n">
         <v>1211.2</v>
       </c>
-      <c r="J10" t="n">
+      <c r="K10" t="n">
         <v>0.1806570625439214</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr"/>
-      <c r="B11" t="n">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>SJM</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr"/>
+      <c r="C11" t="n">
         <v>-2.4</v>
       </c>
-      <c r="C11" t="n">
+      <c r="D11" t="n">
         <v>12159000000</v>
       </c>
-      <c r="D11" t="n">
+      <c r="E11" t="n">
         <v>117.1</v>
       </c>
-      <c r="E11" t="n">
+      <c r="F11" t="n">
         <v>0.27</v>
       </c>
-      <c r="F11" t="n">
+      <c r="G11" t="n">
         <v>1224627</v>
       </c>
-      <c r="G11" t="n">
+      <c r="H11" t="n">
         <v>3.69</v>
       </c>
-      <c r="H11" t="n">
+      <c r="I11" t="n">
         <v>98.77</v>
       </c>
-      <c r="I11" t="n">
+      <c r="J11" t="n">
         <v>127.59</v>
       </c>
-      <c r="J11" t="n">
+      <c r="K11" t="n">
         <v>0.6360166551006243</v>
       </c>
     </row>
@@ -2552,7 +2772,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2563,368 +2783,423 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>Ticker</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>P/E Ratio</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>EPS</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Market Cap</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Current Price</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Beta</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Volume</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Dividend Yield</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>52 Week Low</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>52 Week High</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>Momentum Score</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>AAPL</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
         <v>35.05</v>
       </c>
-      <c r="B2" t="n">
+      <c r="C2" t="n">
         <v>6.3</v>
       </c>
-      <c r="C2" t="n">
+      <c r="D2" t="n">
         <v>3317000000000</v>
       </c>
-      <c r="D2" t="n">
+      <c r="E2" t="n">
         <v>227.48</v>
       </c>
-      <c r="E2" t="n">
+      <c r="F2" t="n">
         <v>1.18</v>
       </c>
-      <c r="F2" t="n">
+      <c r="G2" t="n">
         <v>52766532</v>
       </c>
-      <c r="G2" t="n">
+      <c r="H2" t="n">
         <v>0.44</v>
       </c>
-      <c r="H2" t="n">
+      <c r="I2" t="n">
         <v>164.08</v>
       </c>
-      <c r="I2" t="n">
+      <c r="J2" t="n">
         <v>260.1</v>
       </c>
-      <c r="J2" t="n">
+      <c r="K2" t="n">
         <v>0.6602791085190582</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>MSFT</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
         <v>30.71</v>
       </c>
-      <c r="B3" t="n">
+      <c r="C3" t="n">
         <v>12.39</v>
       </c>
-      <c r="C3" t="n">
+      <c r="D3" t="n">
         <v>2828000000000</v>
       </c>
-      <c r="D3" t="n">
+      <c r="E3" t="n">
         <v>380.16</v>
       </c>
-      <c r="E3" t="n">
+      <c r="F3" t="n">
         <v>0.91</v>
       </c>
-      <c r="F3" t="n">
+      <c r="G3" t="n">
         <v>23030403</v>
       </c>
-      <c r="G3" t="n">
+      <c r="H3" t="n">
         <v>0.87</v>
       </c>
-      <c r="H3" t="n">
+      <c r="I3" t="n">
         <v>376.91</v>
       </c>
-      <c r="I3" t="n">
+      <c r="J3" t="n">
         <v>468.35</v>
       </c>
-      <c r="J3" t="n">
+      <c r="K3" t="n">
         <v>0.03554243219597551</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>NVDA</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
         <v>36.99</v>
       </c>
-      <c r="B4" t="n">
+      <c r="C4" t="n">
         <v>2.94</v>
       </c>
-      <c r="C4" t="n">
+      <c r="D4" t="n">
         <v>2654000000000</v>
       </c>
-      <c r="D4" t="n">
+      <c r="E4" t="n">
         <v>106.98</v>
       </c>
-      <c r="E4" t="n">
+      <c r="F4" t="n">
         <v>1.76</v>
       </c>
-      <c r="F4" t="n">
+      <c r="G4" t="n">
         <v>268910687</v>
       </c>
-      <c r="G4" t="n">
+      <c r="H4" t="n">
         <v>0.04</v>
       </c>
-      <c r="H4" t="n">
+      <c r="I4" t="n">
         <v>75.61</v>
       </c>
-      <c r="I4" t="n">
+      <c r="J4" t="n">
         <v>153.13</v>
       </c>
-      <c r="J4" t="n">
+      <c r="K4" t="n">
         <v>0.404669762641899</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="n">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>AMZN</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
         <v>35.61</v>
       </c>
-      <c r="B5" t="n">
+      <c r="C5" t="n">
         <v>5.52</v>
       </c>
-      <c r="C5" t="n">
+      <c r="D5" t="n">
         <v>2083000000000</v>
       </c>
-      <c r="D5" t="n">
+      <c r="E5" t="n">
         <v>194.54</v>
       </c>
-      <c r="E5" t="n">
+      <c r="F5" t="n">
         <v>1.19</v>
       </c>
-      <c r="F5" t="n">
+      <c r="G5" t="n">
         <v>38216186</v>
       </c>
-      <c r="G5" t="inlineStr"/>
-      <c r="H5" t="n">
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="n">
         <v>151.61</v>
       </c>
-      <c r="I5" t="n">
+      <c r="J5" t="n">
         <v>242.52</v>
       </c>
-      <c r="J5" t="n">
+      <c r="K5" t="n">
         <v>0.4722252777472223</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="n">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>GOOGL</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
         <v>20.4</v>
       </c>
-      <c r="B6" t="n">
+      <c r="C6" t="n">
         <v>8.039999999999999</v>
       </c>
-      <c r="C6" t="n">
+      <c r="D6" t="n">
         <v>2010000000000</v>
       </c>
-      <c r="D6" t="n">
+      <c r="E6" t="n">
         <v>165.87</v>
       </c>
-      <c r="E6" t="n">
+      <c r="F6" t="n">
         <v>1.02</v>
       </c>
-      <c r="F6" t="n">
+      <c r="G6" t="n">
         <v>29760381</v>
       </c>
-      <c r="G6" t="n">
+      <c r="H6" t="n">
         <v>0.48</v>
       </c>
-      <c r="H6" t="n">
+      <c r="I6" t="n">
         <v>138.99</v>
       </c>
-      <c r="I6" t="n">
+      <c r="J6" t="n">
         <v>207.05</v>
       </c>
-      <c r="J6" t="n">
+      <c r="K6" t="n">
         <v>0.3949456362033499</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="n">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>META</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
         <v>25.39</v>
       </c>
-      <c r="B7" t="n">
+      <c r="C7" t="n">
         <v>23.86</v>
       </c>
-      <c r="C7" t="n">
+      <c r="D7" t="n">
         <v>1535000000000</v>
       </c>
-      <c r="D7" t="n">
+      <c r="E7" t="n">
         <v>597.99</v>
       </c>
-      <c r="E7" t="n">
+      <c r="F7" t="n">
         <v>1.23</v>
       </c>
-      <c r="F7" t="n">
+      <c r="G7" t="n">
         <v>15379791</v>
       </c>
-      <c r="G7" t="n">
+      <c r="H7" t="n">
         <v>0.35</v>
       </c>
-      <c r="H7" t="n">
+      <c r="I7" t="n">
         <v>414.5</v>
       </c>
-      <c r="I7" t="n">
+      <c r="J7" t="n">
         <v>740.91</v>
       </c>
-      <c r="J7" t="n">
+      <c r="K7" t="n">
         <v>0.5621457675929047</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="n">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>AVGO</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
         <v>88</v>
       </c>
-      <c r="B8" t="n">
+      <c r="C8" t="n">
         <v>2.16</v>
       </c>
-      <c r="C8" t="n">
+      <c r="D8" t="n">
         <v>893790000000</v>
       </c>
-      <c r="D8" t="n">
+      <c r="E8" t="n">
         <v>184.45</v>
       </c>
-      <c r="E8" t="n">
+      <c r="F8" t="n">
         <v>1.03</v>
       </c>
-      <c r="F8" t="n">
+      <c r="G8" t="n">
         <v>36359712</v>
       </c>
-      <c r="G8" t="n">
+      <c r="H8" t="n">
         <v>1.28</v>
       </c>
-      <c r="H8" t="n">
+      <c r="I8" t="n">
         <v>119.76</v>
       </c>
-      <c r="I8" t="n">
+      <c r="J8" t="n">
         <v>251.88</v>
       </c>
-      <c r="J8" t="n">
+      <c r="K8" t="n">
         <v>0.4896306388132</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="n">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>TSLA</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
         <v>113.03</v>
       </c>
-      <c r="B9" t="n">
+      <c r="C9" t="n">
         <v>2.04</v>
       </c>
-      <c r="C9" t="n">
+      <c r="D9" t="n">
         <v>741665000000</v>
       </c>
-      <c r="D9" t="n">
+      <c r="E9" t="n">
         <v>222.15</v>
       </c>
-      <c r="E9" t="n">
+      <c r="F9" t="n">
         <v>2.51</v>
       </c>
-      <c r="F9" t="n">
+      <c r="G9" t="n">
         <v>88969515</v>
       </c>
-      <c r="G9" t="inlineStr"/>
-      <c r="H9" t="n">
+      <c r="H9" t="inlineStr"/>
+      <c r="I9" t="n">
         <v>138.8</v>
       </c>
-      <c r="I9" t="n">
+      <c r="J9" t="n">
         <v>488.54</v>
       </c>
-      <c r="J9" t="n">
+      <c r="K9" t="n">
         <v>0.2383198947789786</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="n">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>WMT</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
         <v>36.28</v>
       </c>
-      <c r="B10" t="n">
+      <c r="C10" t="n">
         <v>2.41</v>
       </c>
-      <c r="C10" t="n">
+      <c r="D10" t="n">
         <v>702440000000</v>
       </c>
-      <c r="D10" t="n">
+      <c r="E10" t="n">
         <v>87.81999999999999</v>
       </c>
-      <c r="E10" t="n">
+      <c r="F10" t="n">
         <v>0.54</v>
       </c>
-      <c r="F10" t="n">
+      <c r="G10" t="n">
         <v>18920062</v>
       </c>
-      <c r="G10" t="n">
+      <c r="H10" t="n">
         <v>1.07</v>
       </c>
-      <c r="H10" t="n">
+      <c r="I10" t="n">
         <v>58.56</v>
       </c>
-      <c r="I10" t="n">
+      <c r="J10" t="n">
         <v>105.3</v>
       </c>
-      <c r="J10" t="n">
+      <c r="K10" t="n">
         <v>0.6260162601626015</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="n">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>JPM</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
         <v>11.61</v>
       </c>
-      <c r="B11" t="n">
+      <c r="C11" t="n">
         <v>19.74</v>
       </c>
-      <c r="C11" t="n">
+      <c r="D11" t="n">
         <v>640701000000</v>
       </c>
-      <c r="D11" t="n">
+      <c r="E11" t="n">
         <v>232.22</v>
       </c>
-      <c r="E11" t="n">
+      <c r="F11" t="n">
         <v>1.09</v>
       </c>
-      <c r="F11" t="n">
+      <c r="G11" t="n">
         <v>10007600</v>
       </c>
-      <c r="G11" t="n">
+      <c r="H11" t="n">
         <v>2.15</v>
       </c>
-      <c r="H11" t="n">
+      <c r="I11" t="n">
         <v>179.2</v>
       </c>
-      <c r="I11" t="n">
+      <c r="J11" t="n">
         <v>280.25</v>
       </c>
-      <c r="J11" t="n">
+      <c r="K11" t="n">
         <v>0.5246907471548738</v>
       </c>
     </row>

</xml_diff>